<commit_message>
Ajuste na rotina pra melhorar o caso do dia 27-02
</commit_message>
<xml_diff>
--- a/casos_aprovados/caso_2026_02_27/input.xlsx
+++ b/casos_aprovados/caso_2026_02_27/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\waljo\projetos\roteirizador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E339D2AB-22E4-4487-AC9C-BA79EC4EAF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A74F5D-28F9-43A7-9FED-4EB376F6FD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-135" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="B1:H57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -660,7 +660,7 @@
       <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="6">
         <v>0.2986111111111111</v>
       </c>
       <c r="E12" s="10"/>
@@ -835,7 +835,9 @@
       <c r="B27" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
       <c r="D27" s="2">
         <v>3</v>
       </c>

</xml_diff>